<commit_message>
modified the Date_Template file
</commit_message>
<xml_diff>
--- a/docs/Data_Template.xlsx
+++ b/docs/Data_Template.xlsx
@@ -1,24 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27809"/>
+  <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lsd/Documents/ghw2018_web_portal_inlandwater_co2/docs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="option_menus" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$C$2:$R$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">main!$C$2:$W$4</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="118">
   <si>
     <t>Site Information</t>
   </si>
@@ -116,9 +129,6 @@
     <t>Floodplain</t>
   </si>
   <si>
-    <t>Others (please specify in the UserNote column)</t>
-  </si>
-  <si>
     <t>Decimal Degree</t>
   </si>
   <si>
@@ -131,12 +141,6 @@
     <t>Altitude</t>
   </si>
   <si>
-    <t>Meter</t>
-  </si>
-  <si>
-    <t>feet</t>
-  </si>
-  <si>
     <t>mm-dd-yyyy</t>
   </si>
   <si>
@@ -271,6 +275,73 @@
   </si>
   <si>
     <r>
+      <t>km</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> yr</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <t>m3 s-1</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>decimal degree</t>
+  </si>
+  <si>
+    <t>inch</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>mile</t>
+  </si>
+  <si>
+    <t>#Fill in cell where it applies.</t>
+  </si>
+  <si>
+    <t>m2</t>
+  </si>
+  <si>
+    <r>
       <t>m</t>
     </r>
     <r>
@@ -282,17 +353,60 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> d</t>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>km</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ft</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>mile</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ft s</t>
     </r>
     <r>
       <rPr>
@@ -307,8 +421,31 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>L d</t>
+    <t>Wind Velocity</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <r>
+      <t>°</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12.65"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>C</t>
+    </r>
+  </si>
+  <si>
+    <t>°F</t>
+  </si>
+  <si>
+    <r>
+      <t>cm s</t>
     </r>
     <r>
       <rPr>
@@ -323,29 +460,36 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>ft</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> d</t>
+    <t>°C</t>
+  </si>
+  <si>
+    <r>
+      <t>CO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Gas Concentration</t>
+  </si>
+  <si>
+    <t>µatm</t>
+  </si>
+  <si>
+    <t>ppm</t>
+  </si>
+  <si>
+    <r>
+      <t>µmol L</t>
     </r>
     <r>
       <rPr>
@@ -361,28 +505,7 @@
   </si>
   <si>
     <r>
-      <t>m</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> hr</t>
+      <t>nmol L</t>
     </r>
     <r>
       <rPr>
@@ -398,137 +521,11 @@
   </si>
   <si>
     <r>
-      <t>L hr</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ft</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> hr</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>km</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> yr</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-  </si>
-  <si>
-    <t>m3 s-1</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>cm</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>meter</t>
-  </si>
-  <si>
-    <t>decimal degree</t>
-  </si>
-  <si>
-    <t>inch</t>
-  </si>
-  <si>
-    <t>km</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>mile</t>
-  </si>
-  <si>
-    <t>#Fill in cell where it applies.</t>
-  </si>
-  <si>
-    <t>m2</t>
-  </si>
-  <si>
-    <r>
-      <t>m</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
+      <t>CO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -537,185 +534,6 @@
       </rPr>
       <t>2</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>km</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ft</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>mile</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>ft s</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-  </si>
-  <si>
-    <t>Wind Velocity</t>
-  </si>
-  <si>
-    <t>Temperature</t>
-  </si>
-  <si>
-    <r>
-      <t>°</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12.65"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>C</t>
-    </r>
-  </si>
-  <si>
-    <t>°F</t>
-  </si>
-  <si>
-    <r>
-      <t>cm s</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-  </si>
-  <si>
-    <t>°C</t>
-  </si>
-  <si>
-    <r>
-      <t>CO</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <t>Gas Concentration</t>
-  </si>
-  <si>
-    <t>µatm</t>
-  </si>
-  <si>
-    <t>ppm</t>
-  </si>
-  <si>
-    <r>
-      <t>µmol L</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>nmol L</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>CO</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -725,22 +543,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> Flux</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>k</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>600</t>
     </r>
   </si>
   <si>
@@ -1106,51 +908,333 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>meq L</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+    <t>µg L-1</t>
+  </si>
+  <si>
+    <r>
+      <t>µg L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>-1</t>
     </r>
   </si>
   <si>
-    <t>µg L-1</t>
-  </si>
-  <si>
-    <r>
-      <t>µg L</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+    <t>UserNote</t>
+  </si>
+  <si>
+    <t>Estuary</t>
+  </si>
+  <si>
+    <r>
+      <t>CH</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>O</t>
+    </r>
+  </si>
+  <si>
+    <t>Others (please specify.)</t>
+  </si>
+  <si>
+    <t>foot</t>
+  </si>
+  <si>
+    <r>
+      <t>mmol L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
       </rPr>
       <t>-1</t>
     </r>
   </si>
   <si>
-    <t>UserNote</t>
-  </si>
-  <si>
-    <t>Estuary</t>
+    <r>
+      <t>CH</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Flux</t>
+    </r>
+  </si>
+  <si>
+    <t>mg N m-2 d-1</t>
+  </si>
+  <si>
+    <t>mg N m-2 hr-1</t>
+  </si>
+  <si>
+    <t>µg N m-2 s-1</t>
+  </si>
+  <si>
+    <t>g N m-2 yr-1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>O</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Flux</t>
+    </r>
+  </si>
+  <si>
+    <t>nmol L-1</t>
+  </si>
+  <si>
+    <t>ft</t>
+  </si>
+  <si>
+    <r>
+      <t>k-CO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>k-CH</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>k-N</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>O</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>-CO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>-CH</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>-N</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>O</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1220,6 +1304,39 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1356,10 +1473,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1372,9 +1493,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1407,9 +1525,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1427,7 +1542,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1489,9 +1608,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1524,9 +1643,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1730,297 +1849,361 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z13"/>
+  <dimension ref="A1:AG13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="18" customWidth="1"/>
-    <col min="4" max="5" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" style="2" customWidth="1"/>
-    <col min="12" max="12" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="9.140625" style="3"/>
-    <col min="21" max="23" width="9.140625" style="2"/>
-    <col min="24" max="24" width="13.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.140625" style="2"/>
-    <col min="26" max="26" width="9.140625" style="5"/>
-    <col min="27" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="22.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" style="16" customWidth="1"/>
+    <col min="4" max="5" width="16.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" style="4" customWidth="1"/>
+    <col min="16" max="16" width="9" style="4" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="16.33203125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="12" style="4" customWidth="1"/>
+    <col min="20" max="20" width="15.83203125" style="5" customWidth="1"/>
+    <col min="21" max="23" width="11.83203125" style="2" customWidth="1"/>
+    <col min="24" max="26" width="10.5" style="2" customWidth="1"/>
+    <col min="27" max="27" width="8.83203125" style="3"/>
+    <col min="28" max="30" width="8.83203125" style="2"/>
+    <col min="31" max="31" width="13.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.83203125" style="2"/>
+    <col min="33" max="33" width="8.83203125" style="5"/>
+    <col min="34" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
+    <row r="1" spans="1:33" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" s="20"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="21"/>
+    </row>
+    <row r="3" spans="1:33" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="P4" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="R2" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="S2" s="22"/>
-      <c r="T2" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="23"/>
+      <c r="Q4" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="U4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="V4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="W4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="X4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA4" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB4" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC4" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF4" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG4" s="11" t="s">
+        <v>95</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="17"/>
-      <c r="C3" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="V3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="X3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>23</v>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C5" s="16" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q4" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="T4" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="U4" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="V4" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y4" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="Z4" s="12" t="s">
-        <v>108</v>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C6" s="16" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C5" s="18" t="s">
-        <v>24</v>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C7" s="16" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C6" s="18" t="s">
-        <v>25</v>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C8" s="16" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C7" s="18" t="s">
-        <v>26</v>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C9" s="16" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C8" s="18" t="s">
-        <v>27</v>
-      </c>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C9" s="18" t="s">
-        <v>28</v>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C11" s="16" t="s">
+        <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C10" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C12" s="16" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C11" s="18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C12" s="18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C13" s="18" t="s">
-        <v>32</v>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="C13" s="16" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <dataConsolidate/>
+  <mergeCells count="6">
     <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:O2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:Z2"/>
+    <mergeCell ref="G2:N2"/>
+    <mergeCell ref="AA2:AG2"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="U2:Z2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2058,13 +2241,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
           <x14:formula1>
-            <xm:f>option_menus!$F$2:$F$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>G4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
-          <x14:formula1>
-            <xm:f>option_menus!$G$2:$G$4</xm:f>
+            <xm:f>option_menus!$G$2:$G$5</xm:f>
           </x14:formula1>
           <xm:sqref>H4</xm:sqref>
         </x14:dataValidation>
@@ -2074,77 +2251,83 @@
           </x14:formula1>
           <xm:sqref>I4</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down list.">
+          <x14:formula1>
+            <xm:f>option_menus!$J$2:$J$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>K4</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
+          <x14:formula1>
+            <xm:f>option_menus!$K$2:$K$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>L4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>option_menus!$L$2:$L$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>M4:N4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
+          <x14:formula1>
+            <xm:f>option_menus!$M$2:$M$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>O4:Q4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
+          <x14:formula1>
+            <xm:f>option_menus!$N$2:$N$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>R4:S4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
+          <x14:formula1>
+            <xm:f>option_menus!$P$2:$P$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>U4:Z4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
+          <x14:formula1>
+            <xm:f>option_menus!$Q$2:$Q$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>AA4:AC4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
+          <x14:formula1>
+            <xm:f>option_menus!$R$2:$R$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>AE4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
+          <x14:formula1>
+            <xm:f>option_menus!$S$2:$S$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>AF4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
+          <x14:formula1>
+            <xm:f>option_menus!$T$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>AG4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
+          <x14:formula1>
+            <xm:f>option_menus!$F$2:$F$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>G4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down list.">
           <x14:formula1>
             <xm:f>option_menus!$I$2:$I$5</xm:f>
           </x14:formula1>
           <xm:sqref>J4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down list.">
-          <x14:formula1>
-            <xm:f>option_menus!$J$2:$J$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>K4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down list.">
-          <x14:formula1>
-            <xm:f>option_menus!$K$2:$K$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>L4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
-          <x14:formula1>
-            <xm:f>option_menus!$L$2:$L$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>M4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>option_menus!$M$2:$M$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>N4:O4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
-          <x14:formula1>
-            <xm:f>option_menus!$N$2:$N$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>P4</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
           <x14:formula1>
             <xm:f>option_menus!$O$2:$O$8</xm:f>
           </x14:formula1>
-          <xm:sqref>Q4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
-          <x14:formula1>
-            <xm:f>option_menus!$P$2:$P$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>R4:S4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
-          <x14:formula1>
-            <xm:f>option_menus!$Q$2:$Q$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>T4:V4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
-          <x14:formula1>
-            <xm:f>option_menus!$R$2:$R$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>X4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
-          <x14:formula1>
-            <xm:f>option_menus!$S$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>Y4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select from the drop down menu.">
-          <x14:formula1>
-            <xm:f>option_menus!$T$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>Z4</xm:sqref>
+          <xm:sqref>T4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2154,25 +2337,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="4" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" customWidth="1"/>
+    <col min="18" max="18" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2180,46 +2364,46 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>17</v>
@@ -2234,7 +2418,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2242,235 +2426,230 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="H2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I2" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="J2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="N2" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="O2" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="P2" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q2" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="R2" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="S2" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="T2" s="19" t="s">
-        <v>109</v>
+        <v>45</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="T2" s="17" t="s">
+        <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="H3" t="s">
         <v>61</v>
       </c>
       <c r="I3" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="J3" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="K3" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="L3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="M3" t="s">
-        <v>79</v>
-      </c>
-      <c r="N3" t="s">
-        <v>85</v>
-      </c>
-      <c r="O3" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="P3" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q3" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="N3" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="O3" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="S3" t="s">
         <v>103</v>
       </c>
-      <c r="R3" t="s">
-        <v>107</v>
-      </c>
     </row>
-    <row r="4" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="G4" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="H4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="S4" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>38</v>
-      </c>
-      <c r="I4" t="s">
-        <v>73</v>
-      </c>
-      <c r="J4" t="s">
-        <v>51</v>
-      </c>
-      <c r="K4" t="s">
-        <v>80</v>
-      </c>
-      <c r="L4" t="s">
-        <v>80</v>
-      </c>
-      <c r="N4" t="s">
-        <v>86</v>
-      </c>
-      <c r="O4" s="19" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>41</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
       </c>
+      <c r="F5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" t="s">
+        <v>54</v>
+      </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I5" t="s">
-        <v>74</v>
-      </c>
-      <c r="J5" t="s">
-        <v>55</v>
-      </c>
-      <c r="N5" t="s">
-        <v>87</v>
-      </c>
-      <c r="O5" s="19" t="s">
-        <v>95</v>
+        <v>49</v>
+      </c>
+      <c r="M5" t="s">
+        <v>76</v>
+      </c>
+      <c r="N5" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="O5" s="17" t="s">
+        <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
-      </c>
-      <c r="J6" t="s">
-        <v>56</v>
-      </c>
-      <c r="O6" s="19" t="s">
-        <v>96</v>
+        <v>98</v>
+      </c>
+      <c r="N6" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
         <v>29</v>
       </c>
-      <c r="J7" t="s">
-        <v>57</v>
-      </c>
-      <c r="O7" s="19" t="s">
-        <v>97</v>
+      <c r="N7" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="O7" s="17" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="J8" t="s">
-        <v>52</v>
-      </c>
-      <c r="O8" s="19" t="s">
-        <v>98</v>
+      <c r="N8" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="O8" s="17" t="s">
+        <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="J9" t="s">
-        <v>53</v>
-      </c>
     </row>
-    <row r="10" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="J11" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>